<commit_message>
first scenario completed (simplified version)
</commit_message>
<xml_diff>
--- a/the_carrefour/doc/carrefour data collection.xlsx
+++ b/the_carrefour/doc/carrefour data collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\the_carrefour\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F5A068-C0AB-40AB-9539-5A428559D673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A1CF32-1887-49D7-9149-D780D4BB647E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2985" yWindow="3015" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEST 3" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
   <si>
     <t>data collection at Carrefour San Giuliano Terme</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>TEST 3</t>
+  </si>
+  <si>
+    <t>AVG</t>
   </si>
 </sst>
 </file>
@@ -123,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +151,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -161,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -174,6 +183,8 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -907,10 +918,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{785EF536-0FBE-4240-A3CE-9D59537A6013}">
-  <dimension ref="A2:B15"/>
+  <dimension ref="A2:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,6 +1009,15 @@
         <v>14.51</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="11">
+        <f>MEDIAN(B3:B15)</f>
+        <v>44.29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>